<commit_message>
Tests réalisés sur 1D
</commit_message>
<xml_diff>
--- a/CudaPerf_Thibaut.xlsx
+++ b/CudaPerf_Thibaut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="460" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="460" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="K1 - blocs 1D" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>CUDA de base sur 1 GPU (accés coalescents)</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Gflops</t>
+  </si>
+  <si>
+    <t>55.94</t>
   </si>
   <si>
     <r>
@@ -856,7 +859,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1110,10 +1113,10 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>58.26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>57.77</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v/>
@@ -1207,16 +1210,16 @@
                   <c:v>54.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>58.42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>60.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>60.36</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v/>
@@ -1313,13 +1316,13 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>59.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>61.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>61.16</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v/>
@@ -1416,13 +1419,13 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>68.16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>60.42</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>60.53</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1522,10 +1525,10 @@
                   <c:v>45.78</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>60.27</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v/>
@@ -1622,13 +1625,13 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>20.23</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>46.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>70.94</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2078,12 +2081,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="82288521"/>
-        <c:axId val="20823158"/>
-        <c:axId val="44294198"/>
+        <c:axId val="46629397"/>
+        <c:axId val="59793576"/>
+        <c:axId val="26352196"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="82288521"/>
+        <c:axId val="46629397"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2100,14 +2103,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20823158"/>
+        <c:crossAx val="59793576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20823158"/>
+        <c:axId val="59793576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,11 +2134,11 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82288521"/>
+        <c:crossAx val="46629397"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="44294198"/>
+        <c:axId val="26352196"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2152,7 +2155,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20823158"/>
+        <c:crossAx val="59793576"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2191,7 +2194,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2300,11 +2303,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="150"/>
-        <c:axId val="23621356"/>
-        <c:axId val="90078283"/>
+        <c:axId val="27299793"/>
+        <c:axId val="618853"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="23621356"/>
+        <c:axId val="27299793"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,14 +2324,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="90078283"/>
+        <c:crossAx val="618853"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90078283"/>
+        <c:axId val="618853"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2378,7 +2381,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23621356"/>
+        <c:crossAx val="27299793"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2478,8 +2481,8 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="C25:M35 H9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2570,13 +2573,23 @@
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
       <c r="H9" s="11" t="n">
-        <v>4.73</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+        <v>4.76</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <v>3.91</v>
+      </c>
+      <c r="K9" s="11" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="L9" s="11" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>3.74</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="12" t="s">
@@ -2588,13 +2601,23 @@
       <c r="F10" s="9"/>
       <c r="G10" s="10"/>
       <c r="H10" s="11" t="n">
-        <v>29.02</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+        <v>28.88</v>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>36.77</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <v>35.19</v>
+      </c>
+      <c r="K10" s="11" t="n">
+        <v>35.63</v>
+      </c>
+      <c r="L10" s="11" t="n">
+        <v>36.11</v>
+      </c>
+      <c r="M10" s="11" t="n">
+        <v>36.74</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2617,8 +2640,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25:M35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2754,8 +2777,12 @@
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
+      <c r="K11" s="22" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="L11" s="22" t="n">
+        <v>2.38</v>
+      </c>
       <c r="M11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,10 +2797,18 @@
       <c r="G12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
+      <c r="H12" s="22" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="I12" s="22" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="J12" s="22" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="K12" s="22" t="n">
+        <v>2.28</v>
+      </c>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
     </row>
@@ -2789,9 +2824,15 @@
       <c r="G13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="H13" s="22" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="I13" s="22" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="J13" s="22" t="n">
+        <v>2.25</v>
+      </c>
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
@@ -2806,10 +2847,14 @@
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="22" t="n">
-        <v>2.458</v>
-      </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+        <v>2.02</v>
+      </c>
+      <c r="H14" s="22" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="I14" s="22" t="n">
+        <v>2.27</v>
+      </c>
       <c r="J14" s="23"/>
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
@@ -2826,8 +2871,12 @@
       <c r="F15" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="G15" s="22" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="H15" s="22" t="n">
+        <v>2.28</v>
+      </c>
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
@@ -2841,11 +2890,15 @@
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="E16" s="21" t="n">
+        <v>6.79</v>
+      </c>
       <c r="F16" s="22" t="n">
         <v>2.95</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="22" t="n">
+        <v>1.94</v>
+      </c>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
@@ -3015,8 +3068,12 @@
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
+      <c r="K26" s="22" t="n">
+        <v>58.26</v>
+      </c>
+      <c r="L26" s="22" t="n">
+        <v>57.77</v>
+      </c>
       <c r="M26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3031,10 +3088,18 @@
       <c r="G27" s="22" t="n">
         <v>54.2</v>
       </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
+      <c r="H27" s="22" t="n">
+        <v>53</v>
+      </c>
+      <c r="I27" s="22" t="n">
+        <v>58.42</v>
+      </c>
+      <c r="J27" s="22" t="n">
+        <v>60.3</v>
+      </c>
+      <c r="K27" s="22" t="n">
+        <v>60.36</v>
+      </c>
       <c r="L27" s="23"/>
       <c r="M27" s="23"/>
     </row>
@@ -3047,10 +3112,18 @@
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="G28" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="22" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="I28" s="22" t="n">
+        <v>61.2</v>
+      </c>
+      <c r="J28" s="22" t="n">
+        <v>61.16</v>
+      </c>
       <c r="K28" s="23"/>
       <c r="L28" s="23"/>
       <c r="M28" s="23"/>
@@ -3064,9 +3137,15 @@
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
+      <c r="G29" s="22" t="n">
+        <v>68.16</v>
+      </c>
+      <c r="H29" s="22" t="n">
+        <v>60.42</v>
+      </c>
+      <c r="I29" s="22" t="n">
+        <v>60.53</v>
+      </c>
       <c r="J29" s="23"/>
       <c r="K29" s="23"/>
       <c r="L29" s="23"/>
@@ -3083,8 +3162,12 @@
       <c r="F30" s="22" t="n">
         <v>45.78</v>
       </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
+      <c r="G30" s="22" t="n">
+        <v>70</v>
+      </c>
+      <c r="H30" s="22" t="n">
+        <v>60.27</v>
+      </c>
       <c r="I30" s="23"/>
       <c r="J30" s="23"/>
       <c r="K30" s="23"/>
@@ -3098,11 +3181,15 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="E31" s="21" t="n">
+        <v>20.23</v>
+      </c>
       <c r="F31" s="22" t="n">
         <v>46.64</v>
       </c>
-      <c r="G31" s="22"/>
+      <c r="G31" s="22" t="n">
+        <v>70.94</v>
+      </c>
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
       <c r="J31" s="23"/>
@@ -3210,8 +3297,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="C25:M35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3221,12 +3308,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>10</v>
@@ -3775,8 +3862,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="1" sqref="C25:M35 E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3791,12 +3878,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3812,7 +3899,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
@@ -3822,13 +3909,13 @@
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3873,8 +3960,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="1" sqref="C25:M35 L16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3890,7 +3977,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3906,7 +3993,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -3921,33 +4008,33 @@
         <v>8</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="39"/>
@@ -3966,10 +4053,10 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36"/>
       <c r="C8" s="37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="39"/>
@@ -3991,10 +4078,10 @@
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36"/>
       <c r="C9" s="37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="39"/>
@@ -4019,10 +4106,10 @@
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="36"/>
       <c r="C10" s="41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="42"/>
       <c r="F10" s="43"/>
@@ -4047,13 +4134,13 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="47" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="49"/>
       <c r="F11" s="50"/>
@@ -4067,10 +4154,10 @@
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="47"/>
       <c r="C12" s="53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="54"/>

</xml_diff>

<commit_message>
Algo optimisé : moins de travail dans le vide
</commit_message>
<xml_diff>
--- a/CudaPerf_Thibaut.xlsx
+++ b/CudaPerf_Thibaut.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="460" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="460" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="K1 - blocs 1D" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>CUDA de base sur 1 GPU (accés coalescents)</t>
   </si>
@@ -39,13 +39,13 @@
     </r>
   </si>
   <si>
-    <t>Côté des matrices : </t>
+    <t>Côté des matrices :</t>
   </si>
   <si>
     <t>Utilisez bien des matrices de 4096x4096 pour vos benchs!!</t>
   </si>
   <si>
-    <t>Machine : </t>
+    <t>Machine :</t>
   </si>
   <si>
     <t>Zones à mesurer en premier</t>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Rappel : 1024 threads maximum par bloc</t>
-  </si>
-  <si>
-    <t>Machine :</t>
   </si>
   <si>
     <t>Taille du bloc en Y</t>
@@ -139,6 +136,27 @@
     </r>
   </si>
   <si>
+    <t>veut pas </t>
+  </si>
+  <si>
+    <t>1.972390</t>
+  </si>
+  <si>
+    <t>1.379269</t>
+  </si>
+  <si>
+    <t>1.315034</t>
+  </si>
+  <si>
+    <t>69.681419</t>
+  </si>
+  <si>
+    <t>99.646202</t>
+  </si>
+  <si>
+    <t>104.513634</t>
+  </si>
+  <si>
     <t>CUBLAS</t>
   </si>
   <si>
@@ -267,7 +285,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -314,15 +332,15 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="14"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -345,12 +363,6 @@
     <font>
       <b val="true"/>
       <sz val="14.4"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -566,7 +578,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -607,10 +619,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -623,10 +631,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -776,10 +780,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -873,7 +873,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1400">
+              <a:rPr b="1" sz="1400">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2081,12 +2081,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="46629397"/>
-        <c:axId val="59793576"/>
-        <c:axId val="26352196"/>
+        <c:axId val="98461176"/>
+        <c:axId val="91691066"/>
+        <c:axId val="23136370"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="46629397"/>
+        <c:axId val="98461176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,14 +2103,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="59793576"/>
+        <c:crossAx val="91691066"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59793576"/>
+        <c:axId val="91691066"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2134,11 +2134,11 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46629397"/>
+        <c:crossAx val="98461176"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="26352196"/>
+        <c:axId val="23136370"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2155,8 +2155,8 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="59793576"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="91691066"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2303,11 +2303,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="150"/>
-        <c:axId val="27299793"/>
-        <c:axId val="618853"/>
+        <c:axId val="7558570"/>
+        <c:axId val="90980480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="27299793"/>
+        <c:axId val="7558570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2324,14 +2324,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="618853"/>
+        <c:crossAx val="90980480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="618853"/>
+        <c:axId val="90980480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,7 +2381,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27299793"/>
+        <c:crossAx val="7558570"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2409,15 +2409,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>617400</xdr:colOff>
+      <xdr:colOff>644400</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>617040</xdr:colOff>
+      <xdr:colOff>643680</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>116280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2425,8 +2425,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3043080" y="6905880"/>
-        <a:ext cx="7314840" cy="4571640"/>
+        <a:off x="3032280" y="6896880"/>
+        <a:ext cx="7314480" cy="4571280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2444,15 +2444,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>703440</xdr:colOff>
+      <xdr:colOff>730440</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>417240</xdr:colOff>
+      <xdr:colOff>443880</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2460,8 +2460,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5277240" y="2891160"/>
-        <a:ext cx="7679160" cy="3767040"/>
+        <a:off x="5304240" y="2882160"/>
+        <a:ext cx="7678800" cy="3766680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2481,7 +2481,7 @@
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -2571,51 +2571,51 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11" t="n">
+      <c r="G9" s="9"/>
+      <c r="H9" s="10" t="n">
         <v>4.76</v>
       </c>
-      <c r="I9" s="11" t="n">
+      <c r="I9" s="10" t="n">
         <v>3.74</v>
       </c>
-      <c r="J9" s="11" t="n">
+      <c r="J9" s="10" t="n">
         <v>3.91</v>
       </c>
-      <c r="K9" s="11" t="n">
+      <c r="K9" s="10" t="n">
         <v>3.86</v>
       </c>
-      <c r="L9" s="11" t="n">
+      <c r="L9" s="10" t="n">
         <v>3.81</v>
       </c>
-      <c r="M9" s="11" t="n">
+      <c r="M9" s="10" t="n">
         <v>3.74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11" t="n">
+      <c r="G10" s="9"/>
+      <c r="H10" s="10" t="n">
         <v>28.88</v>
       </c>
-      <c r="I10" s="11" t="n">
+      <c r="I10" s="10" t="n">
         <v>36.77</v>
       </c>
-      <c r="J10" s="11" t="n">
+      <c r="J10" s="10" t="n">
         <v>35.19</v>
       </c>
-      <c r="K10" s="11" t="n">
+      <c r="K10" s="10" t="n">
         <v>35.63</v>
       </c>
-      <c r="L10" s="11" t="n">
+      <c r="L10" s="10" t="n">
         <v>36.11</v>
       </c>
-      <c r="M10" s="11" t="n">
+      <c r="M10" s="10" t="n">
         <v>36.74</v>
       </c>
     </row>
@@ -2647,6 +2647,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
@@ -2676,41 +2677,38 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="3"/>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="14"/>
-    </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="7" t="n">
         <v>1</v>
       </c>
@@ -2746,262 +2744,262 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>12</v>
+      <c r="A10" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22" t="n">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20" t="n">
         <v>2.36</v>
       </c>
-      <c r="L11" s="22" t="n">
+      <c r="L11" s="20" t="n">
         <v>2.38</v>
       </c>
-      <c r="M11" s="23"/>
+      <c r="M11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="22" t="n">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="20" t="n">
         <v>2.59</v>
       </c>
-      <c r="I12" s="22" t="n">
+      <c r="I12" s="20" t="n">
         <v>2.35</v>
       </c>
-      <c r="J12" s="22" t="n">
+      <c r="J12" s="20" t="n">
         <v>2.28</v>
       </c>
-      <c r="K12" s="22" t="n">
+      <c r="K12" s="20" t="n">
         <v>2.28</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="22" t="n">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="20" t="n">
         <v>2.31</v>
       </c>
-      <c r="I13" s="22" t="n">
+      <c r="I13" s="20" t="n">
         <v>2.46</v>
       </c>
-      <c r="J13" s="22" t="n">
+      <c r="J13" s="20" t="n">
         <v>2.25</v>
       </c>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22" t="n">
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20" t="n">
         <v>2.02</v>
       </c>
-      <c r="H14" s="22" t="n">
+      <c r="H14" s="20" t="n">
         <v>2.27</v>
       </c>
-      <c r="I14" s="22" t="n">
+      <c r="I14" s="20" t="n">
         <v>2.27</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="7" t="n">
         <v>32</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22" t="n">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="22" t="n">
+      <c r="G15" s="20" t="n">
         <v>1.96</v>
       </c>
-      <c r="H15" s="22" t="n">
+      <c r="H15" s="20" t="n">
         <v>2.28</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21" t="n">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19" t="n">
         <v>6.79</v>
       </c>
-      <c r="F16" s="22" t="n">
+      <c r="F16" s="20" t="n">
         <v>2.95</v>
       </c>
-      <c r="G16" s="22" t="n">
+      <c r="G16" s="20" t="n">
         <v>1.94</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="7" t="n">
         <v>128</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22" t="n">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20" t="n">
         <v>8.51</v>
       </c>
-      <c r="F17" s="22" t="n">
+      <c r="F17" s="20" t="n">
         <v>2.83</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="7" t="n">
         <v>256</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22" t="n">
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20" t="n">
         <v>8.97</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="7" t="n">
         <v>512</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="7" t="n">
         <v>1024</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17" t="s">
+      <c r="A23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="7" t="n">
         <v>1</v>
       </c>
@@ -3037,239 +3035,239 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="s">
-        <v>12</v>
+      <c r="A25" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="22" t="n">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20" t="n">
         <v>58.26</v>
       </c>
-      <c r="L26" s="22" t="n">
+      <c r="L26" s="20" t="n">
         <v>57.77</v>
       </c>
-      <c r="M26" s="23"/>
+      <c r="M26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22" t="n">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20" t="n">
         <v>54.2</v>
       </c>
-      <c r="H27" s="22" t="n">
+      <c r="H27" s="20" t="n">
         <v>53</v>
       </c>
-      <c r="I27" s="22" t="n">
+      <c r="I27" s="20" t="n">
         <v>58.42</v>
       </c>
-      <c r="J27" s="22" t="n">
+      <c r="J27" s="20" t="n">
         <v>60.3</v>
       </c>
-      <c r="K27" s="22" t="n">
+      <c r="K27" s="20" t="n">
         <v>60.36</v>
       </c>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="22" t="n">
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="20" t="n">
         <v>59.5</v>
       </c>
-      <c r="I28" s="22" t="n">
+      <c r="I28" s="20" t="n">
         <v>61.2</v>
       </c>
-      <c r="J28" s="22" t="n">
+      <c r="J28" s="20" t="n">
         <v>61.16</v>
       </c>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22" t="n">
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="20" t="n">
         <v>68.16</v>
       </c>
-      <c r="H29" s="22" t="n">
+      <c r="H29" s="20" t="n">
         <v>60.42</v>
       </c>
-      <c r="I29" s="22" t="n">
+      <c r="I29" s="20" t="n">
         <v>60.53</v>
       </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="7" t="n">
         <v>32</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22" t="n">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20" t="n">
         <v>45.78</v>
       </c>
-      <c r="G30" s="22" t="n">
+      <c r="G30" s="20" t="n">
         <v>70</v>
       </c>
-      <c r="H30" s="22" t="n">
+      <c r="H30" s="20" t="n">
         <v>60.27</v>
       </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="20"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21" t="n">
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19" t="n">
         <v>20.23</v>
       </c>
-      <c r="F31" s="22" t="n">
+      <c r="F31" s="20" t="n">
         <v>46.64</v>
       </c>
-      <c r="G31" s="22" t="n">
+      <c r="G31" s="20" t="n">
         <v>70.94</v>
       </c>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="7" t="n">
         <v>128</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22" t="n">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20" t="n">
         <v>16.14</v>
       </c>
-      <c r="F32" s="22" t="n">
+      <c r="F32" s="20" t="n">
         <v>48.5</v>
       </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="20"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="7" t="n">
         <v>256</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22" t="n">
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="20" t="n">
         <v>15.33</v>
       </c>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="20"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="7" t="n">
         <v>512</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="20"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="7" t="n">
         <v>1024</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3297,8 +3295,8 @@
   </sheetPr>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3308,12 +3306,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>10</v>
@@ -3337,36 +3335,33 @@
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="3"/>
-      <c r="I5" s="13"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="14"/>
-    </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="7" t="n">
         <v>1</v>
       </c>
@@ -3402,216 +3397,224 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>12</v>
+      <c r="A10" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18"/>
       <c r="B13" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18"/>
       <c r="B14" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18"/>
       <c r="B15" s="7" t="n">
         <v>32</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="7" t="n">
         <v>128</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="7" t="n">
         <v>256</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="7" t="n">
         <v>512</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="7" t="n">
         <v>1024</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="17" t="s">
+      <c r="A23" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="7" t="n">
         <v>1</v>
       </c>
@@ -3647,193 +3650,201 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="20" t="s">
-        <v>12</v>
+      <c r="A25" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="18"/>
       <c r="B28" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="18"/>
       <c r="B29" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="18"/>
       <c r="B30" s="7" t="n">
         <v>32</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="20"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="7" t="n">
         <v>128</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="20"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="7" t="n">
         <v>256</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="20"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="7" t="n">
         <v>512</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="20"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="7" t="n">
         <v>1024</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3878,12 +3889,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3899,42 +3910,42 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>24</v>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="B10" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3977,7 +3988,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3993,7 +4004,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
@@ -4001,172 +4012,172 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>31</v>
+      <c r="G6" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="10" t="n">
+      <c r="B7" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="10" t="e">
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="9" t="e">
         <f aca="false">F7/F11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L7" s="26"/>
+      <c r="L7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="10" t="e">
+      <c r="B8" s="34"/>
+      <c r="C8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="9" t="e">
         <f aca="false">F8/F7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="10" t="n">
+      <c r="I8" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="10" t="e">
+      <c r="J8" s="24"/>
+      <c r="K8" s="9" t="e">
         <f aca="false">F8/F11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L8" s="26"/>
+      <c r="L8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="36"/>
-      <c r="C9" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="10" t="e">
+      <c r="B9" s="34"/>
+      <c r="C9" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="9" t="e">
         <f aca="false">F9/F7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I9" s="10" t="e">
+      <c r="I9" s="9" t="e">
         <f aca="false">F9/F8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9" s="10" t="n">
+      <c r="J9" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K9" s="10" t="e">
+      <c r="K9" s="9" t="e">
         <f aca="false">F9/F11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L9" s="26"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="36"/>
-      <c r="C10" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="45" t="e">
+      <c r="B10" s="34"/>
+      <c r="C10" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="43" t="e">
         <f aca="false">F10/F7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="45" t="e">
+      <c r="I10" s="43" t="e">
         <f aca="false">F10/F8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="45" t="e">
+      <c r="J10" s="43" t="e">
         <f aca="false">F10/F9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="46"/>
-      <c r="L10" s="45" t="e">
+      <c r="K10" s="44"/>
+      <c r="L10" s="43" t="e">
         <f aca="false">F10/F12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
+      <c r="B11" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="47"/>
-      <c r="C12" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>